<commit_message>
Update skor peer review
</commit_message>
<xml_diff>
--- a/My_Professional_Reviews/18222087_UAS-5_Skor.xlsx
+++ b/My_Professional_Reviews/18222087_UAS-5_Skor.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Satria\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Satria\Documents\STEI\Komunikasi Interpersonal\all-about-me\My_Professional_Reviews\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907540AB-B64F-4376-B5DF-19FC1799EE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33EDCC69-8879-4FE6-8D0E-05FE5DE31E32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{8AFE3614-8754-EB4D-B44F-1C12FCF6F8C2}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>Fikrifalah Muslich</t>
+  </si>
+  <si>
+    <t>Antania Hanjani Yustika Putri</t>
   </si>
 </sst>
 </file>
@@ -526,7 +529,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -657,9 +660,27 @@
       <c r="AP3" s="4"/>
     </row>
     <row r="4" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="G4" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A4" s="2">
+        <v>18224083</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="2">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2">
+        <v>5</v>
+      </c>
+      <c r="E4" s="2">
+        <v>4</v>
+      </c>
+      <c r="F4" s="2">
+        <v>5</v>
+      </c>
+      <c r="G4" s="4">
+        <f t="shared" si="0"/>
+        <v>4.75</v>
       </c>
       <c r="L4" s="4"/>
       <c r="Q4" s="4"/>
@@ -1736,7 +1757,7 @@
   <dimension ref="A1:AP82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1867,9 +1888,27 @@
       <c r="AP3" s="4"/>
     </row>
     <row r="4" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="G4" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A4" s="2">
+        <v>18224083</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="2">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2">
+        <v>5</v>
+      </c>
+      <c r="E4" s="2">
+        <v>4</v>
+      </c>
+      <c r="F4" s="2">
+        <v>4</v>
+      </c>
+      <c r="G4" s="4">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
       </c>
       <c r="L4" s="4"/>
       <c r="Q4" s="4"/>
@@ -2945,7 +2984,7 @@
   <dimension ref="A1:AP82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3076,9 +3115,27 @@
       <c r="AP3" s="4"/>
     </row>
     <row r="4" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="G4" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A4" s="2">
+        <v>18224083</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="2">
+        <v>4</v>
+      </c>
+      <c r="D4" s="2">
+        <v>5</v>
+      </c>
+      <c r="E4" s="2">
+        <v>5</v>
+      </c>
+      <c r="F4" s="2">
+        <v>5</v>
+      </c>
+      <c r="G4" s="4">
+        <f t="shared" si="0"/>
+        <v>4.75</v>
       </c>
       <c r="L4" s="4"/>
       <c r="Q4" s="4"/>
@@ -4285,9 +4342,27 @@
       <c r="AP3" s="4"/>
     </row>
     <row r="4" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="G4" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A4" s="2">
+        <v>18224083</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="2">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2">
+        <v>5</v>
+      </c>
+      <c r="E4" s="2">
+        <v>5</v>
+      </c>
+      <c r="F4" s="2">
+        <v>4</v>
+      </c>
+      <c r="G4" s="4">
+        <f t="shared" si="0"/>
+        <v>4.75</v>
       </c>
       <c r="L4" s="4"/>
       <c r="Q4" s="4"/>

</xml_diff>

<commit_message>
Update Skor UAS again
</commit_message>
<xml_diff>
--- a/My_Professional_Reviews/18222087_UAS-5_Skor.xlsx
+++ b/My_Professional_Reviews/18222087_UAS-5_Skor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Satria\Documents\STEI\Komunikasi Interpersonal\all-about-me\My_Professional_Reviews\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6AB42B-5E2C-42CE-B001-2DB04E3AEDCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13EDBEFE-7AA1-4FF3-901D-191355600889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{8AFE3614-8754-EB4D-B44F-1C12FCF6F8C2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{8AFE3614-8754-EB4D-B44F-1C12FCF6F8C2}"/>
   </bookViews>
   <sheets>
     <sheet name="UAS_1_My_Concepts" sheetId="2" r:id="rId1"/>
@@ -525,11 +525,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B73929F8-86DE-C24C-A270-AE251CD40D12}">
   <dimension ref="A1:AP82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4210,7 +4210,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D1F948-1ADF-4B33-979B-06CD398BC5BF}">
   <dimension ref="A1:AP82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>

</xml_diff>